<commit_message>
asked about concerns every day vs not every day
</commit_message>
<xml_diff>
--- a/Call4Concern(1-59) (anonymised) v3.xlsx
+++ b/Call4Concern(1-59) (anonymised) v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f1751b608ea6aab/Business/Medicine/QIP/Escalation to ICU/Report/Data/escalation_to_icu_analysis_2/escalation_to_icu_qip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\escalation_to_icu\escalation_to_icu_qip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{66B741A3-5789-4468-837A-3222A71B325E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3EC4DAA-1B2F-C643-ACF4-BCA42A86FD4C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747D8BDD-83F4-4613-A130-FB94E4880BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="500" windowWidth="13180" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="18810" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -939,9 +939,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -979,7 +979,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1085,7 +1085,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1227,7 +1227,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1237,13 +1237,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="28.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" ht="80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1415,10 +1415,10 @@
         <v>33</v>
       </c>
       <c r="AH2" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1501,10 +1501,10 @@
         <v>33</v>
       </c>
       <c r="AH3" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1679,10 +1679,10 @@
         <v>33</v>
       </c>
       <c r="AH5" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1872,10 +1872,10 @@
         <v>33</v>
       </c>
       <c r="AH7" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1970,10 +1970,10 @@
         <v>33</v>
       </c>
       <c r="AH8" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2068,10 +2068,10 @@
         <v>33</v>
       </c>
       <c r="AH9" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2335,10 +2335,10 @@
         <v>37</v>
       </c>
       <c r="AH12" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2412,10 +2412,10 @@
         <v>37</v>
       </c>
       <c r="AH13" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5067,7 +5067,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>

</xml_diff>